<commit_message>
changed col names in this new excel
</commit_message>
<xml_diff>
--- a/res/test_data/erdri/erdri_cds_funny_column_names.xlsx
+++ b/res/test_data/erdri/erdri_cds_funny_column_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Documents\dataspell\rarelink_phenopacket_mapper\res\test_data\erdri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52EE303-8159-49A1-B458-FA47D3E56368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC529044-E494-423D-AEE6-89B0DEE99837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="13758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="30" windowWidth="17280" windowHeight="9984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>data_type</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>specification</t>
-  </si>
-  <si>
     <t xml:space="preserve">Patient's pseudonym </t>
   </si>
   <si>
@@ -49,9 +34,6 @@
   </si>
   <si>
     <t>1. Pseudonym</t>
-  </si>
-  <si>
-    <t>section</t>
   </si>
   <si>
     <t>2. Personal information</t>
@@ -174,6 +156,24 @@
   </si>
   <si>
     <t>Phenotype (HPO), Genotype (HGVS)</t>
+  </si>
+  <si>
+    <t>section1</t>
+  </si>
+  <si>
+    <t>name__</t>
+  </si>
+  <si>
+    <t>des</t>
+  </si>
+  <si>
+    <t>data_typess</t>
+  </si>
+  <si>
+    <t>necessary</t>
+  </si>
+  <si>
+    <t>spec2</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -507,36 +507,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -544,196 +544,196 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>